<commit_message>
Adding the DREF forecasting capacity
</commit_message>
<xml_diff>
--- a/Taxonomies/IsoContinentRegion.xlsx
+++ b/Taxonomies/IsoContinentRegion.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2439" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2451" uniqueCount="490">
   <si>
     <t xml:space="preserve">ISO Code</t>
   </si>
@@ -1475,6 +1475,12 @@
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XKX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kosovo</t>
   </si>
   <si>
     <r>
@@ -1719,17 +1725,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L207"/>
+  <dimension ref="A1:L208"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C181" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F204" activeCellId="0" sqref="F204:L204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.5"/>
@@ -9455,19 +9461,57 @@
         <v>51</v>
       </c>
     </row>
-    <row r="205" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="3" t="s">
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="1" t="s">
         <v>485</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D204" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F204" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G204" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H204" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I204" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J204" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K204" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L204" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="3" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="4" t="s">
-        <v>487</v>
+      <c r="A207" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="4" t="s">
+        <v>489</v>
       </c>
     </row>
   </sheetData>

</xml_diff>